<commit_message>
tested with new data and removed unnecessary apps
</commit_message>
<xml_diff>
--- a/test/data/pdb_metafile_sample1b.xlsx
+++ b/test/data/pdb_metafile_sample1b.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qzhang/qzwk_dir/qzModules/ProteinStructureUtils/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57C13AC-D7E9-4348-A9CC-BC15F45C81E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC36926A-8F6C-ED49-9B89-F779054E8FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="1480" windowWidth="24640" windowHeight="13520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>Narrative ID</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>JCVISYN3_0004.pdb</t>
+  </si>
+  <si>
+    <t>From RCSB</t>
   </si>
 </sst>
 </file>
@@ -905,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -917,7 +920,7 @@
     <col min="4" max="4" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -933,8 +936,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>50569</v>
       </c>
@@ -950,8 +956,11 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>50569</v>
       </c>
@@ -964,8 +973,11 @@
       <c r="E3" t="s">
         <v>8</v>
       </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>50569</v>
       </c>
@@ -981,8 +993,11 @@
       <c r="E4" t="s">
         <v>12</v>
       </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>50569</v>
       </c>
@@ -996,10 +1011,14 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>